<commit_message>
Karo-búsqueda agregada e UX
</commit_message>
<xml_diff>
--- a/contactosInicial.xlsx
+++ b/contactosInicial.xlsx
@@ -1,34 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol\Downloads\Directorio-py-master\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Álvarez</t>
+  </si>
+  <si>
+    <t>julia.alvarez@gmail.com</t>
+  </si>
+  <si>
+    <t>Luisa</t>
+  </si>
+  <si>
+    <t>Hernández</t>
+  </si>
+  <si>
+    <t>luisa.hernanza@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>Rodríguez</t>
+  </si>
+  <si>
+    <t>camilo.rodri@gmail.com</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Casas</t>
+  </si>
+  <si>
+    <t>p.casas@gmail.com</t>
+  </si>
+  <si>
+    <t>Ángela</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>angela.r@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,15 +97,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,74 +402,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Este</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>es</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>uno</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nuevo</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>en la segunda</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>5161149</v>
+      </c>
+      <c r="D1">
+        <v>3022154659</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>daw</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>daw</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>daw</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>dawda</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>fafa</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4659873</v>
+      </c>
+      <c r="D2">
+        <v>3084531624</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2152426</v>
+      </c>
+      <c r="D3">
+        <v>3105498675</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2356849</v>
+      </c>
+      <c r="D4">
+        <v>3152468975</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2114853</v>
+      </c>
+      <c r="D5">
+        <v>3002586491</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Búsqueda por cualqueir campo de registro
</commit_message>
<xml_diff>
--- a/contactosInicial.xlsx
+++ b/contactosInicial.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,52 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ruiz</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alzate</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>32434233423</v>
+      </c>
+      <c r="D6" t="n">
+        <v>123124314</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Ruiz@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Julia</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ana</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>424324234</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2342342</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Juli@hotmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>